<commit_message>
adding updated cross_tabulation file
</commit_message>
<xml_diff>
--- a/cross_tabulation.xlsx
+++ b/cross_tabulation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anaghalokhande/Documents/research_levine/NIRUDAK-CEA_github/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anaghalokhande/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAB412C5-5042-5040-B700-82684DCC705C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{478C3BFE-B1C2-4A41-B4E7-BAF6947A0D49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19460" xr2:uid="{670C52BE-0416-D447-BAFE-2BC106E62F37}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>True Severe</t>
   </si>
@@ -63,6 +63,45 @@
   </si>
   <si>
     <t>WHO No</t>
+  </si>
+  <si>
+    <t>more sensitive, fewer false negatives</t>
+  </si>
+  <si>
+    <t>correctly classifies No  cases more accurately relative to WHO</t>
+  </si>
+  <si>
+    <t>misses more True Some, both overdiagnoses &amp; underdiagnoses people relative to WHO</t>
+  </si>
+  <si>
+    <t>sensitivity = correctly says you're not in the second 2 columns (given that you have Severe)</t>
+  </si>
+  <si>
+    <t>specificity = correctly says you're not in the second 2 rows (given that you have Severe)</t>
+  </si>
+  <si>
+    <t>adjust parameter — assign DALY to undertreating Some</t>
+  </si>
+  <si>
+    <t>add: one-way sensitivity how bad would penalty have to be for undertreating Some</t>
+  </si>
+  <si>
+    <t>JP: double check variation in age distribution based on model</t>
+  </si>
+  <si>
+    <t>state in assumptions that this is not assigned (AL: circle back and do this after rotations, April even just for learning)</t>
+  </si>
+  <si>
+    <t>emphasize that errors of the models are in the different age groups which affects DALYs</t>
+  </si>
+  <si>
+    <t>why we used different DALYs for death</t>
+  </si>
+  <si>
+    <t>"Branch H" (WHO) — 56.61046 DALYs conditional on death in Branch H</t>
+  </si>
+  <si>
+    <t>"Branch Q" (NIRUDAK) — 46.11102 DALYs conditional on death in Branch Q</t>
   </si>
 </sst>
 </file>
@@ -104,9 +143,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -130,14 +172,14 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>109220</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>666712</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -160,8 +202,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2781300" y="2425700"/>
-          <a:ext cx="10877512" cy="3962400"/>
+          <a:off x="3027680" y="5494020"/>
+          <a:ext cx="10847032" cy="3962400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -470,15 +512,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AEEE9CD-384E-494E-A550-99CE5C261BB9}">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.1640625" customWidth="1"/>
     <col min="11" max="11" width="14.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -580,6 +623,59 @@
         <v>180</v>
       </c>
     </row>
+    <row r="6" spans="1:14" ht="136" x14ac:dyDescent="0.2">
+      <c r="B6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="K8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+      <c r="K9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C14" t="s">
+        <v>18</v>
+      </c>
+      <c r="K14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C15" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>